<commit_message>
add prod config, handle font family
</commit_message>
<xml_diff>
--- a/adg-server/src/main/resources/bidv/ĐƠN MUA HÀNG.xlsx
+++ b/adg-server/src/main/resources/bidv/ĐƠN MUA HÀNG.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luan.phm/engineering/Projects/ADongGroup/adg-services/adg-api/src/main/resources/bidv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luan.phm/engineering/Projects/ADongGroup/adg-services/adg-server/src/main/resources/bidv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E30D3B3-AE5B-EF4A-BABB-2A85C1C62297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F58BEFA-2D8C-3741-9CD4-5BEF65D9EBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19200" yWindow="4060" windowWidth="19200" windowHeight="21140" xr2:uid="{902AB5DA-4E46-2F4A-81F7-9F513CBA2FD9}"/>
   </bookViews>
@@ -362,9 +362,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -377,9 +374,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -392,9 +386,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="41" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -413,6 +404,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -440,41 +464,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -794,7 +794,7 @@
   <dimension ref="A3:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A15" sqref="A15:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -809,111 +809,111 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
     </row>
     <row r="7" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="7" t="s">
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="10" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="7" t="s">
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="7" t="s">
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -924,7 +924,7 @@
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -941,164 +941,152 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="43"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="21"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="20"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="17"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="38">
+      <c r="B17" s="23"/>
+      <c r="C17" s="26">
         <v>0.1</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="30"/>
-      <c r="F17" s="17"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="40" t="s">
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="14"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="36"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="41" t="s">
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="41"/>
-      <c r="F19" s="14"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="41"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="D27" s="25" t="s">
+      <c r="B27" s="33"/>
+      <c r="D27" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="D28" s="24" t="s">
+      <c r="B28" s="32"/>
+      <c r="D28" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E29" s="13"/>
+      <c r="E29" s="11"/>
     </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="A17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="C20:F21"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A5:F7"/>
@@ -1115,6 +1103,18 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="C23:F23"/>
     <mergeCell ref="C25:F25"/>
+    <mergeCell ref="A17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="C20:F21"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C22:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>